<commit_message>
Update pinout plan file.
Reflect actual Arduino mapping.
</commit_message>
<xml_diff>
--- a/planning/ATMega809 Pinout Plan.xlsx
+++ b/planning/ATMega809 Pinout Plan.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akimb\Google Drive\hardware hacking\RPi4 Logic Analyzer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akimb\Documents\PCB CAD Projects\ATMega809 Breakout\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F3D1EB-CE0B-45F5-9D00-068AB3308840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AC1068-B467-4CB5-B885-4EF8B6EF8DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="972" yWindow="1932" windowWidth="21516" windowHeight="13308" xr2:uid="{7436E436-D164-4B7E-BF39-F71A5D05B942}"/>
+    <workbookView xWindow="6672" yWindow="3156" windowWidth="22416" windowHeight="13368" xr2:uid="{7436E436-D164-4B7E-BF39-F71A5D05B942}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphical pinout map" sheetId="2" r:id="rId1"/>
     <sheet name="Planning" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Graphical pinout map'!$A$1:$X$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Graphical pinout map'!$A$1:$X$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="175">
   <si>
     <t>Pin</t>
   </si>
@@ -396,21 +396,9 @@
     <t>GND</t>
   </si>
   <si>
-    <t>RX3</t>
-  </si>
-  <si>
     <t>D6</t>
   </si>
   <si>
-    <t>TX3</t>
-  </si>
-  <si>
-    <t>RX</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -466,9 +454,6 @@
   </si>
   <si>
     <t>4x LUT inputs on Px0..2, output on Px3</t>
-  </si>
-  <si>
-    <t>Timers, PWM, EVENT outputs, etc. distributed throughout</t>
   </si>
   <si>
     <r>
@@ -517,9 +502,6 @@
     <t>A5</t>
   </si>
   <si>
-    <t>A10</t>
-  </si>
-  <si>
     <t>EVOUTA</t>
   </si>
   <si>
@@ -550,15 +532,9 @@
     <t>D12/EVOUTD</t>
   </si>
   <si>
-    <t>26 digital I/O pins available</t>
-  </si>
-  <si>
     <t>VIN: Power to regulator; VDD: Power to MCU (from VIN, VUSB, or thru this pin); VBUS - I2C; VREF - Analog ref.</t>
   </si>
   <si>
-    <t>Serial port</t>
-  </si>
-  <si>
     <t>TWD</t>
   </si>
   <si>
@@ -578,6 +554,68 @@
   </si>
   <si>
     <t>SPI alt. position on PORTE</t>
+  </si>
+  <si>
+    <t>EVENT outputs distributed throughout</t>
+  </si>
+  <si>
+    <t>24 digital I/O pins available</t>
+  </si>
+  <si>
+    <t>Timer/PWM</t>
+  </si>
+  <si>
+    <t>TCA0</t>
+  </si>
+  <si>
+    <t>TCB3</t>
+  </si>
+  <si>
+    <t>TCB2</t>
+  </si>
+  <si>
+    <t>TCA0 PWM output on D10..D15</t>
+  </si>
+  <si>
+    <t>TCB0..3 PWM output on D2, D3, D8, D9</t>
+  </si>
+  <si>
+    <t>RX0</t>
+  </si>
+  <si>
+    <t>TX0</t>
+  </si>
+  <si>
+    <t>RX2</t>
+  </si>
+  <si>
+    <t>TX2</t>
+  </si>
+  <si>
+    <r>
+      <t>Serial port (Arduino HWSERIAL</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -730,7 +768,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -1271,11 +1309,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1430,9 +1503,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1451,9 +1521,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1515,6 +1582,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1840,10 +1934,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB41"/>
+  <dimension ref="A1:AB43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1892,7 +1986,7 @@
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="13" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -1923,7 +2017,7 @@
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="13" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
@@ -1984,16 +2078,16 @@
         <v>0</v>
       </c>
       <c r="C5" s="16"/>
-      <c r="D5" s="76">
+      <c r="D5" s="74">
         <v>16</v>
       </c>
-      <c r="E5" s="77">
+      <c r="E5" s="75">
         <v>15</v>
       </c>
-      <c r="F5" s="77">
+      <c r="F5" s="75">
         <v>14</v>
       </c>
-      <c r="G5" s="82">
+      <c r="G5" s="80">
         <v>13</v>
       </c>
       <c r="H5" s="9">
@@ -2002,7 +2096,7 @@
       <c r="I5" s="19"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
-      <c r="L5" s="86">
+      <c r="L5" s="84">
         <v>11</v>
       </c>
       <c r="M5" s="37">
@@ -2032,7 +2126,7 @@
       <c r="U5" s="25">
         <v>2</v>
       </c>
-      <c r="V5" s="93">
+      <c r="V5" s="91">
         <v>1</v>
       </c>
       <c r="W5" s="9">
@@ -2046,28 +2140,28 @@
     </row>
     <row r="6" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="78" t="s">
+      <c r="D6" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="79" t="s">
+      <c r="E6" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="F6" s="80" t="s">
+      <c r="F6" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="83" t="s">
+      <c r="G6" s="81" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="81" t="s">
+      <c r="H6" s="79" t="s">
         <v>118</v>
       </c>
       <c r="I6" s="19"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
-      <c r="L6" s="84" t="s">
+      <c r="L6" s="82" t="s">
         <v>118</v>
       </c>
       <c r="M6" s="38" t="s">
@@ -2077,10 +2171,10 @@
         <v>65</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="P6" s="27" t="s">
-        <v>121</v>
+        <v>171</v>
       </c>
       <c r="Q6" s="40" t="s">
         <v>64</v>
@@ -2095,10 +2189,10 @@
         <v>51</v>
       </c>
       <c r="U6" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="V6" s="94" t="s">
-        <v>123</v>
+        <v>146</v>
+      </c>
+      <c r="V6" s="92" t="s">
+        <v>145</v>
       </c>
       <c r="W6" s="10" t="s">
         <v>118</v>
@@ -2111,7 +2205,7 @@
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B7" s="14" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="12"/>
@@ -2122,45 +2216,35 @@
       <c r="I7" s="19"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="75" t="s">
+      <c r="L7" s="82"/>
+      <c r="M7" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="N7" s="101" t="s">
+        <v>167</v>
+      </c>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="100" t="s">
         <v>152</v>
       </c>
-      <c r="N7" s="29" t="s">
+      <c r="T7" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="O7" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="P7" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q7" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="R7" s="41"/>
-      <c r="S7" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="T7" s="65" t="s">
-        <v>157</v>
-      </c>
-      <c r="U7" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="V7" s="74" t="s">
-        <v>133</v>
-      </c>
-      <c r="W7" s="68"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="99"/>
+      <c r="W7" s="10"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
       <c r="Z7" s="42"/>
       <c r="AA7" s="42"/>
       <c r="AB7" s="42"/>
     </row>
-    <row r="8" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="12"/>
@@ -2171,67 +2255,83 @@
       <c r="I8" s="19"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="O8" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="P8" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q8" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="R8" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="S8" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="T8" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="U8" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="V8" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="W8" s="8"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="73" t="s">
+        <v>172</v>
+      </c>
+      <c r="N8" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="O8" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q8" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="V8" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="W8" s="67"/>
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
       <c r="Z8" s="42"/>
       <c r="AA8" s="42"/>
       <c r="AB8" s="42"/>
     </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
+    <row r="9" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="P9" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q9" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="R9" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="S9" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="U9" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="V9" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="W9" s="8"/>
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
       <c r="Z9" s="42"/>
@@ -2241,24 +2341,24 @@
     <row r="10" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
       <c r="V10" s="12"/>
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
@@ -2267,95 +2367,59 @@
       <c r="AA10" s="42"/>
       <c r="AB10" s="42"/>
     </row>
-    <row r="11" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
       <c r="Z11" s="42"/>
       <c r="AA11" s="42"/>
       <c r="AB11" s="42"/>
     </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="K12" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="L12" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="M12" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="N12" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="O12" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="P12" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="59" t="s">
-        <v>25</v>
-      </c>
-      <c r="S12" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="T12" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="U12" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="V12" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="W12" s="7"/>
-      <c r="X12" s="20"/>
+    <row r="12" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
       <c r="Z12" s="42"/>
       <c r="AA12" s="42"/>
@@ -2363,57 +2427,63 @@
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C13" s="16"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="69" t="s">
-        <v>163</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="G13" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="H13" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="I13" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="J13" s="54" t="s">
-        <v>146</v>
-      </c>
-      <c r="K13" s="54" t="s">
-        <v>147</v>
-      </c>
-      <c r="L13" s="54" t="s">
-        <v>148</v>
-      </c>
-      <c r="M13" s="54" t="s">
-        <v>153</v>
-      </c>
-      <c r="N13" s="54" t="s">
-        <v>154</v>
-      </c>
-      <c r="O13" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="P13" s="71" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q13" s="72"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="54" t="s">
-        <v>149</v>
-      </c>
-      <c r="U13" s="58" t="s">
-        <v>129</v>
-      </c>
-      <c r="V13" s="73"/>
-      <c r="W13" s="68"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="L13" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="M13" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N13" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="O13" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="P13" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q13" s="61"/>
+      <c r="R13" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="S13" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="T13" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="U13" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="V13" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="W13" s="7"/>
       <c r="X13" s="20"/>
       <c r="Y13" s="12"/>
       <c r="Z13" s="42"/>
@@ -2422,140 +2492,98 @@
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C14" s="16"/>
-      <c r="D14" s="84" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="22" t="s">
+      <c r="D14" s="69"/>
+      <c r="E14" s="68" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="G14" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="I14" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="J14" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="L14" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="M14" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="N14" s="56" t="s">
-        <v>83</v>
-      </c>
-      <c r="O14" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="P14" s="88" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q14" s="89" t="s">
-        <v>118</v>
-      </c>
-      <c r="R14" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="S14" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="T14" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="U14" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="V14" s="91" t="s">
-        <v>75</v>
-      </c>
-      <c r="W14" s="10" t="s">
-        <v>118</v>
-      </c>
+      <c r="I14" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="J14" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="K14" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="L14" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="M14" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="N14" s="54" t="s">
+        <v>148</v>
+      </c>
+      <c r="O14" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="P14" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q14" s="71"/>
+      <c r="R14" s="97"/>
+      <c r="S14" s="96"/>
+      <c r="T14" s="96"/>
+      <c r="U14" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="V14" s="98"/>
+      <c r="W14" s="67"/>
       <c r="X14" s="20"/>
       <c r="Y14" s="12"/>
       <c r="Z14" s="42"/>
       <c r="AA14" s="42"/>
       <c r="AB14" s="42"/>
     </row>
-    <row r="15" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="C15" s="16"/>
-      <c r="D15" s="85">
-        <v>17</v>
-      </c>
-      <c r="E15" s="64">
-        <v>18</v>
-      </c>
-      <c r="F15" s="52">
-        <v>19</v>
-      </c>
-      <c r="G15" s="53">
-        <v>20</v>
-      </c>
-      <c r="H15" s="53">
-        <v>21</v>
-      </c>
-      <c r="I15" s="53">
-        <v>22</v>
-      </c>
-      <c r="J15" s="55">
-        <v>23</v>
-      </c>
-      <c r="K15" s="53">
-        <v>24</v>
-      </c>
-      <c r="L15" s="53">
-        <v>25</v>
-      </c>
-      <c r="M15" s="57">
-        <v>26</v>
-      </c>
-      <c r="N15" s="57">
-        <v>27</v>
-      </c>
-      <c r="O15" s="57">
-        <v>28</v>
-      </c>
-      <c r="P15" s="87">
-        <v>29</v>
-      </c>
-      <c r="Q15" s="90">
-        <v>30</v>
-      </c>
-      <c r="R15" s="62">
-        <v>31</v>
-      </c>
-      <c r="S15" s="55">
-        <v>32</v>
-      </c>
-      <c r="T15" s="55">
-        <v>33</v>
-      </c>
-      <c r="U15" s="55">
-        <v>34</v>
-      </c>
-      <c r="V15" s="92">
-        <v>35</v>
-      </c>
-      <c r="W15" s="11">
-        <v>36</v>
-      </c>
+      <c r="D15" s="69"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="J15" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="K15" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="L15" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="93"/>
+      <c r="Q15" s="94"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="95"/>
+      <c r="W15" s="67"/>
       <c r="X15" s="20"/>
       <c r="Y15" s="12"/>
       <c r="Z15" s="42"/>
@@ -2563,94 +2591,170 @@
       <c r="AB15" s="42"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B16" s="17"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="12"/>
+      <c r="B16" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="82" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="J16" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="N16" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="O16" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="P16" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q16" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="R16" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="S16" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="T16" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="U16" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="V16" s="89" t="s">
+        <v>75</v>
+      </c>
+      <c r="W16" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="X16" s="20"/>
       <c r="Y16" s="12"/>
       <c r="Z16" s="42"/>
       <c r="AA16" s="42"/>
       <c r="AB16" s="42"/>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B17" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
+    <row r="17" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="83">
+        <v>17</v>
+      </c>
+      <c r="E17" s="64">
+        <v>18</v>
+      </c>
+      <c r="F17" s="52">
+        <v>19</v>
+      </c>
+      <c r="G17" s="53">
+        <v>20</v>
+      </c>
+      <c r="H17" s="53">
+        <v>21</v>
+      </c>
+      <c r="I17" s="53">
+        <v>22</v>
+      </c>
+      <c r="J17" s="55">
+        <v>23</v>
+      </c>
+      <c r="K17" s="53">
+        <v>24</v>
+      </c>
+      <c r="L17" s="53">
+        <v>25</v>
+      </c>
+      <c r="M17" s="57">
+        <v>26</v>
+      </c>
+      <c r="N17" s="57">
+        <v>27</v>
+      </c>
+      <c r="O17" s="57">
+        <v>28</v>
+      </c>
+      <c r="P17" s="85">
+        <v>29</v>
+      </c>
+      <c r="Q17" s="88">
+        <v>30</v>
+      </c>
+      <c r="R17" s="62">
+        <v>31</v>
+      </c>
+      <c r="S17" s="55">
+        <v>32</v>
+      </c>
+      <c r="T17" s="55">
+        <v>33</v>
+      </c>
+      <c r="U17" s="55">
+        <v>34</v>
+      </c>
+      <c r="V17" s="90">
+        <v>35</v>
+      </c>
+      <c r="W17" s="11">
+        <v>36</v>
+      </c>
+      <c r="X17" s="20"/>
       <c r="Y17" s="12"/>
       <c r="Z17" s="42"/>
       <c r="AA17" s="42"/>
       <c r="AB17" s="42"/>
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B18" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="R18" s="12"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="12"/>
-      <c r="W18" s="12"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="18"/>
+      <c r="V18" s="18"/>
+      <c r="W18" s="18"/>
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
       <c r="Z18" s="42"/>
@@ -2658,16 +2762,16 @@
       <c r="AB18" s="42"/>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B19" s="46" t="s">
-        <v>165</v>
+      <c r="B19" s="44" t="s">
+        <v>132</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="43" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="43"/>
-      <c r="G19" s="42"/>
+      <c r="G19" s="43"/>
       <c r="H19" s="43"/>
       <c r="I19" s="43"/>
       <c r="J19" s="43"/>
@@ -2677,9 +2781,7 @@
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
-      <c r="Q19" s="15" t="s">
-        <v>143</v>
-      </c>
+      <c r="Q19" s="12"/>
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
       <c r="T19" s="12"/>
@@ -2693,13 +2795,11 @@
       <c r="AB19" s="42"/>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B20" s="47" t="s">
-        <v>135</v>
+      <c r="B20" s="45" t="s">
+        <v>133</v>
       </c>
       <c r="C20" s="20"/>
-      <c r="D20" s="43" t="s">
-        <v>169</v>
-      </c>
+      <c r="D20" s="43"/>
       <c r="E20" s="12"/>
       <c r="F20" s="43"/>
       <c r="G20" s="42"/>
@@ -2712,8 +2812,8 @@
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
-      <c r="Q20" s="12" t="s">
-        <v>144</v>
+      <c r="Q20" s="15" t="s">
+        <v>140</v>
       </c>
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
@@ -2728,12 +2828,12 @@
       <c r="AB20" s="42"/>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B21" s="48" t="s">
-        <v>138</v>
+      <c r="B21" s="46" t="s">
+        <v>157</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="43" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="43"/>
@@ -2747,7 +2847,9 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
+      <c r="Q21" s="15" t="s">
+        <v>162</v>
+      </c>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
       <c r="T21" s="12"/>
@@ -2761,12 +2863,12 @@
       <c r="AB21" s="42"/>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B22" s="49" t="s">
-        <v>139</v>
+      <c r="B22" s="47" t="s">
+        <v>131</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="43" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="43"/>
@@ -2780,7 +2882,9 @@
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
+      <c r="Q22" s="12" t="s">
+        <v>168</v>
+      </c>
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
       <c r="T22" s="12"/>
@@ -2794,12 +2898,12 @@
       <c r="AB22" s="42"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B23" s="50" t="s">
-        <v>141</v>
+      <c r="B23" s="48" t="s">
+        <v>134</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="43" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="43"/>
@@ -2813,15 +2917,15 @@
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
+      <c r="Q23" t="s">
+        <v>169</v>
+      </c>
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
       <c r="T23" s="12"/>
       <c r="U23" s="12"/>
-      <c r="V23" s="67"/>
-      <c r="W23" s="67" t="s">
-        <v>166</v>
-      </c>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
       <c r="X23" s="12"/>
       <c r="Y23" s="12"/>
       <c r="Z23" s="42"/>
@@ -2829,9 +2933,13 @@
       <c r="AB23" s="42"/>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B24" s="18"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="B24" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="43" t="s">
+        <v>136</v>
+      </c>
       <c r="E24" s="12"/>
       <c r="F24" s="43"/>
       <c r="G24" s="42"/>
@@ -2844,7 +2952,9 @@
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
+      <c r="Q24" s="12" t="s">
+        <v>139</v>
+      </c>
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
@@ -2858,17 +2968,21 @@
       <c r="AB24" s="42"/>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="B25" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="43" t="s">
+        <v>138</v>
+      </c>
       <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
       <c r="M25" s="12"/>
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
@@ -2878,8 +2992,10 @@
       <c r="S25" s="12"/>
       <c r="T25" s="12"/>
       <c r="U25" s="12"/>
-      <c r="V25" s="12"/>
-      <c r="W25" s="12"/>
+      <c r="V25" s="66"/>
+      <c r="W25" s="66" t="s">
+        <v>158</v>
+      </c>
       <c r="X25" s="12"/>
       <c r="Y25" s="12"/>
       <c r="Z25" s="42"/>
@@ -2887,59 +3003,59 @@
       <c r="AB25" s="42"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
       <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
+      <c r="G26" s="42"/>
       <c r="H26" s="43"/>
       <c r="I26" s="43"/>
       <c r="J26" s="43"/>
       <c r="K26" s="43"/>
       <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="43"/>
-      <c r="S26" s="43"/>
-      <c r="T26" s="43"/>
-      <c r="U26" s="43"/>
-      <c r="V26" s="43"/>
-      <c r="W26" s="43"/>
-      <c r="X26" s="43"/>
-      <c r="Y26" s="43"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
       <c r="Z26" s="42"/>
       <c r="AA26" s="42"/>
       <c r="AB26" s="42"/>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="43"/>
-      <c r="V27" s="43"/>
-      <c r="W27" s="43"/>
-      <c r="X27" s="43"/>
-      <c r="Y27" s="43"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
       <c r="Z27" s="42"/>
       <c r="AA27" s="42"/>
       <c r="AB27" s="42"/>
@@ -3032,59 +3148,59 @@
       <c r="AB30" s="42"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="42"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="42"/>
-      <c r="S31" s="42"/>
-      <c r="T31" s="42"/>
-      <c r="U31" s="42"/>
-      <c r="V31" s="42"/>
-      <c r="W31" s="42"/>
-      <c r="X31" s="42"/>
-      <c r="Y31" s="42"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="43"/>
+      <c r="T31" s="43"/>
+      <c r="U31" s="43"/>
+      <c r="V31" s="43"/>
+      <c r="W31" s="43"/>
+      <c r="X31" s="43"/>
+      <c r="Y31" s="43"/>
       <c r="Z31" s="42"/>
       <c r="AA31" s="42"/>
       <c r="AB31" s="42"/>
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="42"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="42"/>
-      <c r="T32" s="42"/>
-      <c r="U32" s="42"/>
-      <c r="V32" s="42"/>
-      <c r="W32" s="42"/>
-      <c r="X32" s="42"/>
-      <c r="Y32" s="42"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
+      <c r="T32" s="43"/>
+      <c r="U32" s="43"/>
+      <c r="V32" s="43"/>
+      <c r="W32" s="43"/>
+      <c r="X32" s="43"/>
+      <c r="Y32" s="43"/>
       <c r="Z32" s="42"/>
       <c r="AA32" s="42"/>
       <c r="AB32" s="42"/>
@@ -3350,6 +3466,64 @@
       <c r="AA41" s="42"/>
       <c r="AB41" s="42"/>
     </row>
+    <row r="42" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="42"/>
+      <c r="Q42" s="42"/>
+      <c r="R42" s="42"/>
+      <c r="S42" s="42"/>
+      <c r="T42" s="42"/>
+      <c r="U42" s="42"/>
+      <c r="V42" s="42"/>
+      <c r="W42" s="42"/>
+      <c r="X42" s="42"/>
+      <c r="Y42" s="42"/>
+      <c r="Z42" s="42"/>
+      <c r="AA42" s="42"/>
+      <c r="AB42" s="42"/>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="42"/>
+      <c r="M43" s="42"/>
+      <c r="N43" s="42"/>
+      <c r="O43" s="42"/>
+      <c r="P43" s="42"/>
+      <c r="Q43" s="42"/>
+      <c r="R43" s="42"/>
+      <c r="S43" s="42"/>
+      <c r="T43" s="42"/>
+      <c r="U43" s="42"/>
+      <c r="V43" s="42"/>
+      <c r="W43" s="42"/>
+      <c r="X43" s="42"/>
+      <c r="Y43" s="42"/>
+      <c r="Z43" s="42"/>
+      <c r="AA43" s="42"/>
+      <c r="AB43" s="42"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update pinout to match the Arduino variant specification & add UDPI.
</commit_message>
<xml_diff>
--- a/planning/ATMega809 Pinout Plan.xlsx
+++ b/planning/ATMega809 Pinout Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akimb\Documents\PCB CAD Projects\ATMega809 Breakout\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AC1068-B467-4CB5-B885-4EF8B6EF8DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AC24D4-AB05-4E51-A922-E9C322E5D1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6672" yWindow="3156" windowWidth="22416" windowHeight="13368" xr2:uid="{7436E436-D164-4B7E-BF39-F71A5D05B942}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="180">
   <si>
     <t>Pin</t>
   </si>
@@ -615,6 +615,44 @@
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>UPDI HEADER</t>
+  </si>
+  <si>
+    <t>UPDI</t>
+  </si>
+  <si>
+    <t>N/C</t>
+  </si>
+  <si>
+    <t>but offers ability to power MCU and use serial from programmer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6-pin UPDI Header only </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>requires</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> UPDI and GND pins connected,</t>
     </r>
   </si>
 </sst>
@@ -688,7 +726,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -767,8 +805,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="47">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1344,11 +1388,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1609,6 +1706,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1937,7 +2056,7 @@
   <dimension ref="A1:AB43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1949,8 +2068,7 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="20" width="7.77734375" customWidth="1"/>
     <col min="21" max="21" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="7.77734375" customWidth="1"/>
-    <col min="24" max="24" width="3.6640625" customWidth="1"/>
+    <col min="22" max="24" width="7.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:28" x14ac:dyDescent="0.3">
@@ -2909,9 +3027,9 @@
       <c r="F23" s="43"/>
       <c r="G23" s="42"/>
       <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
       <c r="L23" s="43"/>
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
@@ -2932,7 +3050,7 @@
       <c r="AA23" s="42"/>
       <c r="AB23" s="42"/>
     </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="49" t="s">
         <v>135</v>
       </c>
@@ -2944,9 +3062,11 @@
       <c r="F24" s="43"/>
       <c r="G24" s="42"/>
       <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="103" t="s">
+        <v>175</v>
+      </c>
+      <c r="K24" s="104"/>
       <c r="L24" s="43"/>
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
@@ -2979,10 +3099,14 @@
       <c r="F25" s="43"/>
       <c r="G25" s="42"/>
       <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="105" t="s">
+        <v>176</v>
+      </c>
+      <c r="K25" s="106" t="s">
+        <v>116</v>
+      </c>
+      <c r="L25" s="102"/>
       <c r="M25" s="12"/>
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
@@ -2997,7 +3121,6 @@
         <v>158</v>
       </c>
       <c r="X25" s="12"/>
-      <c r="Y25" s="12"/>
       <c r="Z25" s="42"/>
       <c r="AA25" s="42"/>
       <c r="AB25" s="42"/>
@@ -3010,11 +3133,17 @@
       <c r="F26" s="43"/>
       <c r="G26" s="42"/>
       <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="107" t="s">
+        <v>177</v>
+      </c>
+      <c r="K26" s="108" t="s">
+        <v>146</v>
+      </c>
+      <c r="L26" s="102"/>
+      <c r="M26" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
@@ -3031,7 +3160,7 @@
       <c r="AA26" s="42"/>
       <c r="AB26" s="42"/>
     </row>
-    <row r="27" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
@@ -3039,16 +3168,21 @@
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="109" t="s">
+        <v>145</v>
+      </c>
+      <c r="K27" s="79" t="s">
+        <v>118</v>
+      </c>
+      <c r="L27" s="20"/>
+      <c r="M27" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="N27" s="12"/>
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
+      <c r="R27" s="18"/>
       <c r="S27" s="12"/>
       <c r="T27" s="12"/>
       <c r="U27" s="12"/>
@@ -3525,8 +3659,11 @@
       <c r="AB43" s="42"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J24:K24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="67" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="65" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>